<commit_message>
Switching the div id in grid.js
</commit_message>
<xml_diff>
--- a/data/db-similarity.xlsx
+++ b/data/db-similarity.xlsx
@@ -223,18 +223,18 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -247,11 +247,11 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -577,26 +577,26 @@
       <c r="A3" s="5">
         <v>2.0</v>
       </c>
-      <c r="B3" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="C3" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="D3" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="16">
+      <c r="B3" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="D3" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E3" s="17">
         <v>3.0</v>
       </c>
       <c r="F3" s="9" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H3" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="I3" s="16" t="s">
+      <c r="H3" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="I3" s="17" t="s">
         <v>8</v>
       </c>
     </row>
@@ -604,23 +604,23 @@
       <c r="A4" s="5">
         <v>3.0</v>
       </c>
-      <c r="B4" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="C4" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="D4" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="E4" s="16">
+      <c r="B4" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="E4" s="17">
         <v>3.0</v>
       </c>
       <c r="F4" s="9" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="13">
         <v>2.0</v>
       </c>
       <c r="I4" s="9"/>
@@ -629,23 +629,23 @@
       <c r="A5" s="5">
         <v>4.0</v>
       </c>
-      <c r="B5" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="C5" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="D5" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="E5" s="16">
+      <c r="B5" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="D5" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="E5" s="17">
         <v>2.0</v>
       </c>
       <c r="F5" s="9" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="13">
         <v>3.0</v>
       </c>
       <c r="I5" s="9"/>
@@ -654,16 +654,16 @@
       <c r="A6" s="5">
         <v>5.0</v>
       </c>
-      <c r="B6" s="12">
-        <v>3.0</v>
-      </c>
-      <c r="C6" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="D6" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="E6" s="16">
+      <c r="B6" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="C6" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="D6" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="E6" s="17">
         <v>1.0</v>
       </c>
       <c r="F6" s="9" t="str">
@@ -681,16 +681,16 @@
       <c r="A7" s="5">
         <v>6.0</v>
       </c>
-      <c r="B7" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="C7" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="D7" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="E7" s="16">
+      <c r="B7" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="C7" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="D7" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="E7" s="17">
         <v>1.0</v>
       </c>
       <c r="F7" s="9" t="str">
@@ -702,23 +702,23 @@
       <c r="A8" s="5">
         <v>7.0</v>
       </c>
-      <c r="B8" s="12">
-        <v>3.0</v>
-      </c>
-      <c r="C8" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="D8" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="E8" s="16">
+      <c r="B8" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="C8" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="D8" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="E8" s="17">
         <v>1.0</v>
       </c>
       <c r="F8" s="9" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="15" t="s">
         <v>10</v>
       </c>
     </row>
@@ -726,23 +726,23 @@
       <c r="A9" s="5">
         <v>8.0</v>
       </c>
-      <c r="B9" s="12">
-        <v>3.0</v>
-      </c>
-      <c r="C9" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="D9" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="16">
+      <c r="B9" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="C9" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="17">
         <v>1.0</v>
       </c>
       <c r="F9" s="9" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="15" t="s">
         <v>11</v>
       </c>
     </row>
@@ -750,23 +750,23 @@
       <c r="A10" s="5">
         <v>9.0</v>
       </c>
-      <c r="B10" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="C10" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="D10" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="E10" s="16">
+      <c r="B10" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="C10" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="D10" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="E10" s="17">
         <v>1.0</v>
       </c>
       <c r="F10" s="9" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="15" t="s">
         <v>12</v>
       </c>
     </row>
@@ -774,23 +774,23 @@
       <c r="A11" s="5">
         <v>10.0</v>
       </c>
-      <c r="B11" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="C11" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="D11" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="E11" s="16">
+      <c r="B11" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="D11" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="E11" s="17">
         <v>3.0</v>
       </c>
       <c r="F11" s="9" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="15" t="s">
         <v>13</v>
       </c>
     </row>
@@ -798,16 +798,16 @@
       <c r="A12" s="5">
         <v>11.0</v>
       </c>
-      <c r="B12" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="C12" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="D12" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="E12" s="16">
+      <c r="B12" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="C12" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="D12" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="17">
         <v>3.0</v>
       </c>
       <c r="F12" s="9" t="str">
@@ -819,16 +819,16 @@
       <c r="A13" s="5">
         <v>12.0</v>
       </c>
-      <c r="B13" s="12">
-        <v>3.0</v>
-      </c>
-      <c r="C13" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="D13" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="E13" s="16">
+      <c r="B13" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="C13" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="D13" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="17">
         <v>4.0</v>
       </c>
       <c r="F13" s="9" t="str">
@@ -840,16 +840,16 @@
       <c r="A14" s="5">
         <v>13.0</v>
       </c>
-      <c r="B14" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="C14" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="D14" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="E14" s="16">
+      <c r="B14" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="C14" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="D14" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="E14" s="17">
         <v>1.0</v>
       </c>
       <c r="F14" s="9" t="str">
@@ -861,16 +861,16 @@
       <c r="A15" s="5">
         <v>14.0</v>
       </c>
-      <c r="B15" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="C15" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="D15" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="E15" s="16">
+      <c r="B15" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="C15" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="D15" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="E15" s="17">
         <v>4.0</v>
       </c>
       <c r="F15" s="9" t="str">
@@ -885,16 +885,16 @@
       <c r="B16" s="20">
         <v>3.0</v>
       </c>
-      <c r="C16" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="D16" s="26">
+      <c r="C16" s="24">
+        <v>2.0</v>
+      </c>
+      <c r="D16" s="24">
         <v>1.0</v>
       </c>
       <c r="E16" s="21">
         <v>3.0</v>
       </c>
-      <c r="F16" s="25" t="str">
+      <c r="F16" s="26" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
@@ -981,26 +981,26 @@
       <c r="A3" s="5">
         <v>2.0</v>
       </c>
-      <c r="B3" s="12">
-        <v>3.0</v>
-      </c>
-      <c r="C3" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="E3" s="16">
+      <c r="B3" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="C3" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="E3" s="17">
         <v>4.0</v>
       </c>
       <c r="F3" s="9" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H3" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="I3" s="16" t="s">
+      <c r="H3" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="I3" s="17" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1008,23 +1008,23 @@
       <c r="A4" s="5">
         <v>3.0</v>
       </c>
-      <c r="B4" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="C4" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="D4" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="16">
+      <c r="B4" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="C4" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="D4" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="17">
         <v>4.0</v>
       </c>
       <c r="F4" s="9" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="13">
         <v>2.0</v>
       </c>
       <c r="I4" s="9"/>
@@ -1033,23 +1033,23 @@
       <c r="A5" s="5">
         <v>4.0</v>
       </c>
-      <c r="B5" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="C5" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="D5" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="E5" s="16">
+      <c r="B5" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="D5" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="E5" s="17">
         <v>2.0</v>
       </c>
       <c r="F5" s="9" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="13">
         <v>3.0</v>
       </c>
       <c r="I5" s="9"/>
@@ -1058,16 +1058,16 @@
       <c r="A6" s="5">
         <v>5.0</v>
       </c>
-      <c r="B6" s="12">
-        <v>4.0</v>
-      </c>
-      <c r="C6" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="D6" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="16">
+      <c r="B6" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="C6" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="D6" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="17">
         <v>2.0</v>
       </c>
       <c r="F6" s="9" t="str">
@@ -1085,16 +1085,16 @@
       <c r="A7" s="5">
         <v>6.0</v>
       </c>
-      <c r="B7" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="C7" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="D7" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="E7" s="16">
+      <c r="B7" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="C7" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="D7" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="E7" s="17">
         <v>2.0</v>
       </c>
       <c r="F7" s="9" t="str">
@@ -1106,23 +1106,23 @@
       <c r="A8" s="5">
         <v>7.0</v>
       </c>
-      <c r="B8" s="12">
-        <v>3.0</v>
-      </c>
-      <c r="C8" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="D8" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="E8" s="16">
+      <c r="B8" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="C8" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="D8" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="E8" s="17">
         <v>1.0</v>
       </c>
       <c r="F8" s="9" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="15" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1130,23 +1130,23 @@
       <c r="A9" s="5">
         <v>8.0</v>
       </c>
-      <c r="B9" s="12">
-        <v>4.0</v>
-      </c>
-      <c r="C9" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="D9" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="E9" s="16">
+      <c r="B9" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="C9" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E9" s="17">
         <v>2.0</v>
       </c>
       <c r="F9" s="9" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="15" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1154,23 +1154,23 @@
       <c r="A10" s="5">
         <v>9.0</v>
       </c>
-      <c r="B10" s="12">
-        <v>3.0</v>
-      </c>
-      <c r="C10" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="D10" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="E10" s="16">
+      <c r="B10" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="C10" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="D10" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="E10" s="17">
         <v>1.0</v>
       </c>
       <c r="F10" s="9" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="15" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1178,23 +1178,23 @@
       <c r="A11" s="5">
         <v>10.0</v>
       </c>
-      <c r="B11" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="C11" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="D11" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="E11" s="16">
+      <c r="B11" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="D11" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="E11" s="17">
         <v>4.0</v>
       </c>
       <c r="F11" s="9" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="15" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1202,16 +1202,16 @@
       <c r="A12" s="5">
         <v>11.0</v>
       </c>
-      <c r="B12" s="12">
-        <v>3.0</v>
-      </c>
-      <c r="C12" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="D12" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="E12" s="16">
+      <c r="B12" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="C12" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="D12" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="17">
         <v>2.0</v>
       </c>
       <c r="F12" s="9" t="str">
@@ -1223,16 +1223,16 @@
       <c r="A13" s="5">
         <v>12.0</v>
       </c>
-      <c r="B13" s="12">
-        <v>3.0</v>
-      </c>
-      <c r="C13" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="D13" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="E13" s="16">
+      <c r="B13" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="C13" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="D13" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="17">
         <v>2.0</v>
       </c>
       <c r="F13" s="9" t="str">
@@ -1244,16 +1244,16 @@
       <c r="A14" s="5">
         <v>13.0</v>
       </c>
-      <c r="B14" s="12">
-        <v>3.0</v>
-      </c>
-      <c r="C14" s="14">
-        <v>4.0</v>
-      </c>
-      <c r="D14" s="14">
-        <v>1.0</v>
-      </c>
-      <c r="E14" s="16">
+      <c r="B14" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="C14" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="D14" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E14" s="17">
         <v>2.0</v>
       </c>
       <c r="F14" s="9" t="str">
@@ -1265,16 +1265,16 @@
       <c r="A15" s="5">
         <v>14.0</v>
       </c>
-      <c r="B15" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="C15" s="14">
-        <v>3.0</v>
-      </c>
-      <c r="D15" s="14">
-        <v>2.0</v>
-      </c>
-      <c r="E15" s="16">
+      <c r="B15" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="C15" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="D15" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="E15" s="17">
         <v>4.0</v>
       </c>
       <c r="F15" s="9" t="str">
@@ -1289,16 +1289,16 @@
       <c r="B16" s="20">
         <v>3.0</v>
       </c>
-      <c r="C16" s="26">
-        <v>2.0</v>
-      </c>
-      <c r="D16" s="26">
+      <c r="C16" s="24">
+        <v>2.0</v>
+      </c>
+      <c r="D16" s="24">
         <v>4.0</v>
       </c>
       <c r="E16" s="21">
         <v>1.0</v>
       </c>
-      <c r="F16" s="25" t="str">
+      <c r="F16" s="26" t="str">
         <f t="shared" si="1"/>
         <v>Yes</v>
       </c>
@@ -1360,10 +1360,10 @@
       <c r="A2" s="5">
         <v>1.0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="16"/>
       <c r="F2" s="9" t="str">
         <f t="shared" ref="F2:F16" si="1">IF(COUNTA(B2:E2) = 4, "Yes", "No")</f>
         <v>No</v>
@@ -1385,10 +1385,10 @@
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H3" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="I3" s="16" t="s">
+      <c r="H3" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="I3" s="17" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1404,7 +1404,7 @@
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="13">
         <v>2.0</v>
       </c>
       <c r="I4" s="9"/>
@@ -1421,7 +1421,7 @@
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="13">
         <v>3.0</v>
       </c>
       <c r="I5" s="9"/>
@@ -1470,7 +1470,7 @@
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="15" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1486,7 +1486,7 @@
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="15" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1502,7 +1502,7 @@
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="15" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1518,7 +1518,7 @@
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="15" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1579,10 +1579,10 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="23"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25" t="str">
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26" t="str">
         <f t="shared" si="1"/>
         <v>No</v>
       </c>
@@ -1644,13 +1644,21 @@
       <c r="A2" s="5">
         <v>1.0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="C2" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="D2" s="7">
+        <v>4.0</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1.0</v>
+      </c>
       <c r="F2" s="9" t="str">
         <f t="shared" ref="F2:F16" si="1">IF(COUNTA(B2:E2) = 4, "Yes", "No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>7</v>
@@ -1661,18 +1669,26 @@
       <c r="A3" s="5">
         <v>2.0</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="9"/>
+      <c r="B3" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="C3" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="D3" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="E3" s="17">
+        <v>1.0</v>
+      </c>
       <c r="F3" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-      <c r="H3" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="I3" s="16" t="s">
+        <v>Yes</v>
+      </c>
+      <c r="H3" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="I3" s="17" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1680,15 +1696,23 @@
       <c r="A4" s="5">
         <v>3.0</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="9"/>
+      <c r="B4" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="C4" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="D4" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="E4" s="17">
+        <v>3.0</v>
+      </c>
       <c r="F4" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-      <c r="H4" s="12">
+        <v>Yes</v>
+      </c>
+      <c r="H4" s="13">
         <v>2.0</v>
       </c>
       <c r="I4" s="9"/>
@@ -1697,15 +1721,23 @@
       <c r="A5" s="5">
         <v>4.0</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="9"/>
+      <c r="B5" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="D5" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="E5" s="17">
+        <v>4.0</v>
+      </c>
       <c r="F5" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-      <c r="H5" s="12">
+        <v>Yes</v>
+      </c>
+      <c r="H5" s="13">
         <v>3.0</v>
       </c>
       <c r="I5" s="9"/>
@@ -1714,13 +1746,21 @@
       <c r="A6" s="5">
         <v>5.0</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="9"/>
+      <c r="B6" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="C6" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="D6" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="E6" s="17">
+        <v>1.0</v>
+      </c>
       <c r="F6" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="H6" s="20">
         <v>4.0</v>
@@ -1733,28 +1773,44 @@
       <c r="A7" s="5">
         <v>6.0</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="9"/>
+      <c r="B7" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="C7" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="D7" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="E7" s="17">
+        <v>2.0</v>
+      </c>
       <c r="F7" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5">
         <v>7.0</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="9"/>
+      <c r="B8" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="C8" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="D8" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="17">
+        <v>4.0</v>
+      </c>
       <c r="F8" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-      <c r="H8" s="14" t="s">
+        <v>Yes</v>
+      </c>
+      <c r="H8" s="15" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1762,15 +1818,23 @@
       <c r="A9" s="5">
         <v>8.0</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="9"/>
+      <c r="B9" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="C9" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="D9" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="E9" s="17">
+        <v>1.0</v>
+      </c>
       <c r="F9" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-      <c r="H9" s="14" t="s">
+        <v>Yes</v>
+      </c>
+      <c r="H9" s="15" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1778,15 +1842,23 @@
       <c r="A10" s="5">
         <v>9.0</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="9"/>
+      <c r="B10" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="C10" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="D10" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="E10" s="17">
+        <v>1.0</v>
+      </c>
       <c r="F10" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-      <c r="H10" s="14" t="s">
+        <v>Yes</v>
+      </c>
+      <c r="H10" s="15" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1794,15 +1866,23 @@
       <c r="A11" s="5">
         <v>10.0</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="9"/>
+      <c r="B11" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="D11" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="E11" s="17">
+        <v>4.0</v>
+      </c>
       <c r="F11" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
-      </c>
-      <c r="H11" s="14" t="s">
+        <v>Yes</v>
+      </c>
+      <c r="H11" s="15" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1810,65 +1890,105 @@
       <c r="A12" s="5">
         <v>11.0</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="9"/>
+      <c r="B12" s="13">
+        <v>4.0</v>
+      </c>
+      <c r="C12" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="D12" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="17">
+        <v>2.0</v>
+      </c>
       <c r="F12" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5">
         <v>12.0</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="9"/>
+      <c r="B13" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="C13" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="D13" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="E13" s="17">
+        <v>4.0</v>
+      </c>
       <c r="F13" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="5">
         <v>13.0</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="9"/>
+      <c r="B14" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="C14" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="D14" s="15">
+        <v>4.0</v>
+      </c>
+      <c r="E14" s="17">
+        <v>3.0</v>
+      </c>
       <c r="F14" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5">
         <v>14.0</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="9"/>
+      <c r="B15" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="C15" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="D15" s="15">
+        <v>3.0</v>
+      </c>
+      <c r="E15" s="17">
+        <v>4.0</v>
+      </c>
       <c r="F15" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>No</v>
+        <v>Yes</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="22">
         <v>15.0</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25" t="str">
-        <f t="shared" si="1"/>
-        <v>No</v>
+      <c r="B16" s="20">
+        <v>4.0</v>
+      </c>
+      <c r="C16" s="24">
+        <v>1.0</v>
+      </c>
+      <c r="D16" s="24">
+        <v>2.0</v>
+      </c>
+      <c r="E16" s="21">
+        <v>2.0</v>
+      </c>
+      <c r="F16" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
       </c>
     </row>
   </sheetData>

</xml_diff>